<commit_message>
added Metadata table with notes, ignoring temporary Excel file
</commit_message>
<xml_diff>
--- a/Metadata.xlsx
+++ b/Metadata.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCFA4DC-ACEB-406D-9FE3-682560C5B613}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="304">
   <si>
     <t>key</t>
   </si>
@@ -850,12 +851,93 @@
   </si>
   <si>
     <t>control.settings</t>
+  </si>
+  <si>
+    <t>Photomodul (discontinued)</t>
+  </si>
+  <si>
+    <t>marks protocol as read-only on the device</t>
+  </si>
+  <si>
+    <t>incremental process number on the device</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>raw value</t>
+  </si>
+  <si>
+    <t>calibrated measurement for the filter type in the line (temp_up)</t>
+  </si>
+  <si>
+    <t>system comment for debugging purpose</t>
+  </si>
+  <si>
+    <t>electronic component temperatur OR IF type==F a well volume</t>
+  </si>
+  <si>
+    <t>tells the source reservoir of the pumping</t>
+  </si>
+  <si>
+    <t>feed function parameter (Biolection)</t>
+  </si>
+  <si>
+    <t>Measurement Types</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Environment Parameter</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Fluidics</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>if reservoir==-1 it is the robot</t>
+  </si>
+  <si>
+    <t>Referencing</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Debug Info (deprecated)</t>
+  </si>
+  <si>
+    <t>internally used for BioLector compression mechanism</t>
+  </si>
+  <si>
+    <t>name of calibration file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -865,12 +947,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -885,11 +973,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -905,20 +994,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabelle2" displayName="Tabelle2" ref="A1:H189" totalsRowShown="0">
-  <autoFilter ref="A1:H189"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:H189" totalsRowShown="0">
+  <autoFilter ref="A1:H189" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <sortState ref="A2:H189">
     <sortCondition ref="C1:C189"/>
   </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="key"/>
-    <tableColumn id="7" name="type"/>
-    <tableColumn id="2" name="category"/>
-    <tableColumn id="8" name="comment"/>
-    <tableColumn id="3" name="BL1 table"/>
-    <tableColumn id="4" name="BL1 key"/>
-    <tableColumn id="5" name="BLP group"/>
-    <tableColumn id="6" name="BLP key"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="key"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="type"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="category"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="comment"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="BL1 table"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="BL1 key"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="BLP group"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="BLP key"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1186,22 +1275,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H189"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="C162" sqref="C162"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="4" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
     <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.85546875" customWidth="1"/>
+    <col min="13" max="13" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1396,6 +1487,12 @@
       <c r="C11" t="s">
         <v>193</v>
       </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
       <c r="G11" t="s">
         <v>62</v>
       </c>
@@ -1410,11 +1507,14 @@
       <c r="C12" t="s">
         <v>193</v>
       </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1424,33 +1524,30 @@
       <c r="C13" t="s">
         <v>193</v>
       </c>
-      <c r="D13" t="s">
-        <v>191</v>
-      </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>193</v>
-      </c>
-      <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>26</v>
+        <v>198</v>
+      </c>
+      <c r="G14" t="s">
+        <v>126</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
         <v>198</v>
@@ -1459,7 +1556,7 @@
         <v>126</v>
       </c>
       <c r="H15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1473,7 +1570,7 @@
         <v>126</v>
       </c>
       <c r="H16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
@@ -1487,7 +1584,7 @@
         <v>126</v>
       </c>
       <c r="H17" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1501,7 +1598,7 @@
         <v>126</v>
       </c>
       <c r="H18" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1515,7 +1612,7 @@
         <v>126</v>
       </c>
       <c r="H19" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1529,7 +1626,7 @@
         <v>126</v>
       </c>
       <c r="H20" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1543,7 +1640,7 @@
         <v>126</v>
       </c>
       <c r="H21" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
@@ -1557,7 +1654,7 @@
         <v>126</v>
       </c>
       <c r="H22" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
@@ -1571,7 +1668,7 @@
         <v>126</v>
       </c>
       <c r="H23" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
@@ -1585,7 +1682,7 @@
         <v>126</v>
       </c>
       <c r="H24" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1599,7 +1696,7 @@
         <v>126</v>
       </c>
       <c r="H25" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
@@ -1613,7 +1710,7 @@
         <v>126</v>
       </c>
       <c r="H26" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
@@ -1627,7 +1724,7 @@
         <v>126</v>
       </c>
       <c r="H27" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
@@ -1641,7 +1738,7 @@
         <v>126</v>
       </c>
       <c r="H28" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
@@ -1655,7 +1752,7 @@
         <v>126</v>
       </c>
       <c r="H29" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
@@ -1665,11 +1762,14 @@
       <c r="C30" t="s">
         <v>198</v>
       </c>
+      <c r="D30" t="s">
+        <v>283</v>
+      </c>
       <c r="G30" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="H30" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
@@ -1679,25 +1779,28 @@
       <c r="C31" t="s">
         <v>198</v>
       </c>
+      <c r="D31" t="s">
+        <v>284</v>
+      </c>
       <c r="G31" t="s">
         <v>147</v>
       </c>
       <c r="H31" t="s">
-        <v>158</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C32" t="s">
         <v>198</v>
       </c>
       <c r="G32" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="H32" t="s">
-        <v>164</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
@@ -1705,18 +1808,24 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+      <c r="F33" t="s">
+        <v>32</v>
       </c>
       <c r="G33" t="s">
-        <v>124</v>
+        <v>72</v>
       </c>
       <c r="H33" t="s">
-        <v>125</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
         <v>197</v>
@@ -1725,18 +1834,18 @@
         <v>28</v>
       </c>
       <c r="F34" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
       <c r="G34" t="s">
-        <v>72</v>
+        <v>239</v>
       </c>
       <c r="H34" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C35" t="s">
         <v>197</v>
@@ -1745,18 +1854,18 @@
         <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>86</v>
+        <v>29</v>
       </c>
       <c r="G35" t="s">
         <v>239</v>
       </c>
       <c r="H35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
         <v>197</v>
@@ -1765,47 +1874,47 @@
         <v>28</v>
       </c>
       <c r="F36" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G36" t="s">
         <v>239</v>
       </c>
       <c r="H36" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C37" t="s">
         <v>197</v>
       </c>
-      <c r="E37" t="s">
-        <v>28</v>
-      </c>
-      <c r="F37" t="s">
-        <v>33</v>
-      </c>
       <c r="G37" t="s">
         <v>239</v>
       </c>
       <c r="H37" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
         <v>197</v>
       </c>
+      <c r="E38" t="s">
+        <v>28</v>
+      </c>
+      <c r="F38" t="s">
+        <v>34</v>
+      </c>
       <c r="G38" t="s">
         <v>239</v>
       </c>
       <c r="H38" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
@@ -1815,45 +1924,48 @@
       <c r="C39" t="s">
         <v>197</v>
       </c>
-      <c r="E39" t="s">
-        <v>28</v>
-      </c>
-      <c r="F39" t="s">
-        <v>34</v>
-      </c>
       <c r="G39" t="s">
         <v>239</v>
       </c>
       <c r="H39" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C40" t="s">
         <v>197</v>
       </c>
+      <c r="D40" t="s">
+        <v>303</v>
+      </c>
       <c r="G40" t="s">
         <v>239</v>
       </c>
       <c r="H40" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C41" t="s">
         <v>197</v>
       </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s">
+        <v>37</v>
+      </c>
       <c r="G41" t="s">
-        <v>239</v>
+        <v>62</v>
       </c>
       <c r="H41" t="s">
-        <v>93</v>
+        <v>70</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
@@ -1863,31 +1975,25 @@
       <c r="C42" t="s">
         <v>197</v>
       </c>
-      <c r="E42" t="s">
-        <v>28</v>
-      </c>
-      <c r="F42" t="s">
-        <v>37</v>
-      </c>
       <c r="G42" t="s">
         <v>62</v>
       </c>
       <c r="H42" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C43" t="s">
         <v>197</v>
       </c>
-      <c r="G43" t="s">
-        <v>62</v>
-      </c>
-      <c r="H43" t="s">
-        <v>71</v>
+      <c r="E43" t="s">
+        <v>28</v>
+      </c>
+      <c r="F43" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
@@ -1901,12 +2007,12 @@
         <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
         <v>197</v>
@@ -1915,7 +2021,7 @@
         <v>28</v>
       </c>
       <c r="F45" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
@@ -1929,12 +2035,12 @@
         <v>28</v>
       </c>
       <c r="F46" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C47" t="s">
         <v>197</v>
@@ -1943,7 +2049,7 @@
         <v>28</v>
       </c>
       <c r="F47" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
@@ -1957,7 +2063,7 @@
         <v>28</v>
       </c>
       <c r="F48" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
@@ -1965,33 +2071,42 @@
         <v>25</v>
       </c>
       <c r="C49" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E49" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="F49" t="s">
-        <v>39</v>
+        <v>86</v>
+      </c>
+      <c r="G49" t="s">
+        <v>147</v>
+      </c>
+      <c r="H49" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C50" t="s">
         <v>199</v>
       </c>
+      <c r="D50" t="s">
+        <v>282</v>
+      </c>
       <c r="E50" t="s">
         <v>49</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
+        <v>55</v>
       </c>
       <c r="G50" t="s">
         <v>147</v>
       </c>
       <c r="H50" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
@@ -2001,17 +2116,14 @@
       <c r="C51" t="s">
         <v>199</v>
       </c>
-      <c r="E51" t="s">
-        <v>49</v>
-      </c>
-      <c r="F51" t="s">
-        <v>55</v>
+      <c r="D51" t="s">
+        <v>282</v>
       </c>
       <c r="G51" t="s">
         <v>147</v>
       </c>
       <c r="H51" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
@@ -2025,7 +2137,7 @@
         <v>147</v>
       </c>
       <c r="H52" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
@@ -2039,7 +2151,7 @@
         <v>147</v>
       </c>
       <c r="H53" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
@@ -2049,31 +2161,40 @@
       <c r="C54" t="s">
         <v>199</v>
       </c>
+      <c r="D54" t="s">
+        <v>282</v>
+      </c>
+      <c r="E54" t="s">
+        <v>49</v>
+      </c>
+      <c r="F54" t="s">
+        <v>56</v>
+      </c>
       <c r="G54" t="s">
         <v>147</v>
       </c>
       <c r="H54" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C55" t="s">
-        <v>199</v>
+        <v>97</v>
       </c>
       <c r="E55" t="s">
         <v>49</v>
       </c>
       <c r="F55" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G55" t="s">
         <v>147</v>
       </c>
       <c r="H55" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
@@ -2083,31 +2204,25 @@
       <c r="C56" t="s">
         <v>97</v>
       </c>
-      <c r="E56" t="s">
-        <v>49</v>
-      </c>
-      <c r="F56" t="s">
-        <v>61</v>
-      </c>
       <c r="G56" t="s">
         <v>147</v>
       </c>
       <c r="H56" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C57" t="s">
-        <v>97</v>
+        <v>274</v>
       </c>
       <c r="G57" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="H57" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
@@ -2118,24 +2233,30 @@
         <v>274</v>
       </c>
       <c r="G58" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H58" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C59" t="s">
         <v>274</v>
       </c>
+      <c r="E59" t="s">
+        <v>49</v>
+      </c>
+      <c r="F59" t="s">
+        <v>57</v>
+      </c>
       <c r="G59" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="H59" t="s">
-        <v>120</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
@@ -2145,17 +2266,11 @@
       <c r="C60" t="s">
         <v>274</v>
       </c>
-      <c r="E60" t="s">
-        <v>49</v>
-      </c>
-      <c r="F60" t="s">
-        <v>57</v>
-      </c>
       <c r="G60" t="s">
         <v>147</v>
       </c>
       <c r="H60" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
@@ -2169,7 +2284,7 @@
         <v>147</v>
       </c>
       <c r="H61" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
@@ -2179,11 +2294,17 @@
       <c r="C62" t="s">
         <v>274</v>
       </c>
+      <c r="E62" t="s">
+        <v>49</v>
+      </c>
+      <c r="F62" t="s">
+        <v>58</v>
+      </c>
       <c r="G62" t="s">
         <v>147</v>
       </c>
       <c r="H62" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
@@ -2197,13 +2318,13 @@
         <v>49</v>
       </c>
       <c r="F63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G63" t="s">
         <v>147</v>
       </c>
       <c r="H63" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
@@ -2217,13 +2338,13 @@
         <v>49</v>
       </c>
       <c r="F64" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G64" t="s">
         <v>147</v>
       </c>
       <c r="H64" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
@@ -2233,31 +2354,25 @@
       <c r="C65" t="s">
         <v>274</v>
       </c>
-      <c r="E65" t="s">
-        <v>49</v>
-      </c>
-      <c r="F65" t="s">
-        <v>60</v>
-      </c>
       <c r="G65" t="s">
         <v>147</v>
       </c>
       <c r="H65" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C66" t="s">
         <v>274</v>
       </c>
       <c r="G66" t="s">
-        <v>147</v>
+        <v>107</v>
       </c>
       <c r="H66" t="s">
-        <v>163</v>
+        <v>106</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
@@ -2265,18 +2380,18 @@
         <v>25</v>
       </c>
       <c r="C67" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G67" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="H67" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C68" t="s">
         <v>276</v>
@@ -2285,12 +2400,12 @@
         <v>115</v>
       </c>
       <c r="H68" t="s">
-        <v>116</v>
+        <v>202</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C69" t="s">
         <v>276</v>
@@ -2299,12 +2414,12 @@
         <v>115</v>
       </c>
       <c r="H69" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C70" t="s">
         <v>276</v>
@@ -2313,7 +2428,7 @@
         <v>115</v>
       </c>
       <c r="H70" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="2:8" x14ac:dyDescent="0.25">
@@ -2327,7 +2442,7 @@
         <v>115</v>
       </c>
       <c r="H71" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="2:8" x14ac:dyDescent="0.25">
@@ -2341,7 +2456,7 @@
         <v>115</v>
       </c>
       <c r="H72" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="2:8" x14ac:dyDescent="0.25">
@@ -2355,7 +2470,7 @@
         <v>115</v>
       </c>
       <c r="H73" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="2:8" x14ac:dyDescent="0.25">
@@ -2369,7 +2484,7 @@
         <v>115</v>
       </c>
       <c r="H74" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="75" spans="2:8" x14ac:dyDescent="0.25">
@@ -2383,7 +2498,7 @@
         <v>115</v>
       </c>
       <c r="H75" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="2:8" x14ac:dyDescent="0.25">
@@ -2397,12 +2512,12 @@
         <v>115</v>
       </c>
       <c r="H76" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C77" t="s">
         <v>276</v>
@@ -2411,7 +2526,7 @@
         <v>115</v>
       </c>
       <c r="H77" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
@@ -2425,7 +2540,7 @@
         <v>115</v>
       </c>
       <c r="H78" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
@@ -2439,21 +2554,21 @@
         <v>115</v>
       </c>
       <c r="H79" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C80" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="G80" t="s">
         <v>115</v>
       </c>
       <c r="H80" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="81" spans="2:8" x14ac:dyDescent="0.25">
@@ -2467,7 +2582,7 @@
         <v>115</v>
       </c>
       <c r="H81" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
@@ -2475,13 +2590,13 @@
         <v>23</v>
       </c>
       <c r="C82" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G82" t="s">
         <v>115</v>
       </c>
       <c r="H82" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
@@ -2495,40 +2610,40 @@
         <v>115</v>
       </c>
       <c r="H83" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>23</v>
+        <v>219</v>
       </c>
       <c r="C84" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G84" t="s">
         <v>115</v>
       </c>
       <c r="H84" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>219</v>
+        <v>23</v>
       </c>
       <c r="C85" t="s">
         <v>276</v>
       </c>
       <c r="G85" t="s">
-        <v>115</v>
+        <v>220</v>
       </c>
       <c r="H85" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C86" t="s">
         <v>276</v>
@@ -2537,7 +2652,7 @@
         <v>220</v>
       </c>
       <c r="H86" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -2551,7 +2666,7 @@
         <v>220</v>
       </c>
       <c r="H87" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
@@ -2562,10 +2677,10 @@
         <v>276</v>
       </c>
       <c r="G88" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="H88" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
@@ -2579,7 +2694,7 @@
         <v>224</v>
       </c>
       <c r="H89" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
@@ -2593,26 +2708,26 @@
         <v>224</v>
       </c>
       <c r="H90" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C91" t="s">
         <v>276</v>
       </c>
       <c r="G91" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="H91" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C92" t="s">
         <v>276</v>
@@ -2621,12 +2736,12 @@
         <v>228</v>
       </c>
       <c r="H92" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C93" t="s">
         <v>276</v>
@@ -2635,7 +2750,7 @@
         <v>228</v>
       </c>
       <c r="H93" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
@@ -2649,7 +2764,7 @@
         <v>228</v>
       </c>
       <c r="H94" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
@@ -2663,7 +2778,7 @@
         <v>228</v>
       </c>
       <c r="H95" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
@@ -2677,10 +2792,10 @@
         <v>228</v>
       </c>
       <c r="H96" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="97" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>48</v>
       </c>
@@ -2691,10 +2806,10 @@
         <v>228</v>
       </c>
       <c r="H97" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="98" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>48</v>
       </c>
@@ -2705,41 +2820,41 @@
         <v>228</v>
       </c>
       <c r="H98" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="99" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C99" t="s">
-        <v>276</v>
+        <v>272</v>
+      </c>
+      <c r="D99" t="s">
+        <v>241</v>
       </c>
       <c r="G99" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="H99" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="100" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C100" t="s">
         <v>272</v>
       </c>
-      <c r="D100" t="s">
-        <v>241</v>
-      </c>
       <c r="G100" t="s">
         <v>237</v>
       </c>
       <c r="H100" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="101" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>48</v>
       </c>
@@ -2750,10 +2865,10 @@
         <v>237</v>
       </c>
       <c r="H101" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="102" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>48</v>
       </c>
@@ -2764,10 +2879,10 @@
         <v>237</v>
       </c>
       <c r="H102" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="103" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>48</v>
       </c>
@@ -2778,12 +2893,12 @@
         <v>237</v>
       </c>
       <c r="H103" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="104" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C104" t="s">
         <v>272</v>
@@ -2792,12 +2907,12 @@
         <v>237</v>
       </c>
       <c r="H104" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="105" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C105" t="s">
         <v>272</v>
@@ -2806,10 +2921,10 @@
         <v>237</v>
       </c>
       <c r="H105" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="106" spans="2:8" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="106" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>48</v>
       </c>
@@ -2820,10 +2935,10 @@
         <v>237</v>
       </c>
       <c r="H106" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="107" spans="2:8" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="107" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>48</v>
       </c>
@@ -2834,10 +2949,10 @@
         <v>237</v>
       </c>
       <c r="H107" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="108" spans="2:8" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="108" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>48</v>
       </c>
@@ -2848,10 +2963,13 @@
         <v>237</v>
       </c>
       <c r="H108" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="109" spans="2:8" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="L108" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="109" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>48</v>
       </c>
@@ -2862,12 +2980,18 @@
         <v>237</v>
       </c>
       <c r="H109" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="110" spans="2:8" x14ac:dyDescent="0.25">
+        <v>252</v>
+      </c>
+      <c r="L109" t="s">
+        <v>289</v>
+      </c>
+      <c r="M109" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="110" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C110" t="s">
         <v>272</v>
@@ -2876,10 +3000,16 @@
         <v>237</v>
       </c>
       <c r="H110" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="111" spans="2:8" x14ac:dyDescent="0.25">
+        <v>253</v>
+      </c>
+      <c r="L110" t="s">
+        <v>292</v>
+      </c>
+      <c r="M110" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="111" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>23</v>
       </c>
@@ -2890,12 +3020,18 @@
         <v>237</v>
       </c>
       <c r="H111" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="112" spans="2:8" x14ac:dyDescent="0.25">
+        <v>254</v>
+      </c>
+      <c r="L111" t="s">
+        <v>293</v>
+      </c>
+      <c r="M111" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="112" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C112" t="s">
         <v>272</v>
@@ -2904,26 +3040,41 @@
         <v>237</v>
       </c>
       <c r="H112" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="113" spans="2:8" x14ac:dyDescent="0.25">
+        <v>255</v>
+      </c>
+      <c r="L112" t="s">
+        <v>295</v>
+      </c>
+      <c r="M112" t="s">
+        <v>296</v>
+      </c>
+      <c r="N112" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="113" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C113" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G113" t="s">
         <v>237</v>
       </c>
       <c r="H113" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="114" spans="2:8" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="L113" t="s">
+        <v>297</v>
+      </c>
+      <c r="M113" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="114" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C114" t="s">
         <v>273</v>
@@ -2932,66 +3083,84 @@
         <v>237</v>
       </c>
       <c r="H114" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="115" spans="2:8" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+      <c r="L114" t="s">
+        <v>300</v>
+      </c>
+      <c r="M114" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="115" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C115" t="s">
         <v>273</v>
       </c>
+      <c r="D115" t="s">
+        <v>287</v>
+      </c>
       <c r="G115" t="s">
         <v>237</v>
       </c>
       <c r="H115" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="116" spans="2:8" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="116" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>48</v>
       </c>
       <c r="C116" t="s">
         <v>273</v>
       </c>
+      <c r="D116" t="s">
+        <v>287</v>
+      </c>
       <c r="G116" t="s">
         <v>237</v>
       </c>
       <c r="H116" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="117" spans="2:8" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="117" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>48</v>
       </c>
       <c r="C117" t="s">
         <v>273</v>
       </c>
+      <c r="D117" t="s">
+        <v>287</v>
+      </c>
       <c r="G117" t="s">
         <v>237</v>
       </c>
       <c r="H117" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="118" spans="2:8" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="118" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>48</v>
       </c>
       <c r="C118" t="s">
         <v>273</v>
       </c>
+      <c r="D118" t="s">
+        <v>287</v>
+      </c>
       <c r="G118" t="s">
         <v>237</v>
       </c>
       <c r="H118" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="119" spans="2:8" x14ac:dyDescent="0.25">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="119" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>48</v>
       </c>
@@ -3002,10 +3171,10 @@
         <v>237</v>
       </c>
       <c r="H119" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="120" spans="2:8" x14ac:dyDescent="0.25">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="120" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>48</v>
       </c>
@@ -3016,10 +3185,10 @@
         <v>237</v>
       </c>
       <c r="H120" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="121" spans="2:8" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="121" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>48</v>
       </c>
@@ -3030,12 +3199,12 @@
         <v>237</v>
       </c>
       <c r="H121" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="122" spans="2:8" x14ac:dyDescent="0.25">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="122" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C122" t="s">
         <v>273</v>
@@ -3044,12 +3213,12 @@
         <v>237</v>
       </c>
       <c r="H122" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="123" spans="2:8" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="123" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C123" t="s">
         <v>273</v>
@@ -3058,12 +3227,12 @@
         <v>237</v>
       </c>
       <c r="H123" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="124" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C124" t="s">
         <v>273</v>
@@ -3072,12 +3241,12 @@
         <v>237</v>
       </c>
       <c r="H124" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="125" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C125" t="s">
         <v>273</v>
@@ -3086,10 +3255,10 @@
         <v>237</v>
       </c>
       <c r="H125" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="126" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>48</v>
       </c>
@@ -3100,10 +3269,10 @@
         <v>237</v>
       </c>
       <c r="H126" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="127" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>48</v>
       </c>
@@ -3114,10 +3283,10 @@
         <v>237</v>
       </c>
       <c r="H127" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="128" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>48</v>
       </c>
@@ -3128,7 +3297,7 @@
         <v>237</v>
       </c>
       <c r="H128" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
@@ -3142,21 +3311,21 @@
         <v>237</v>
       </c>
       <c r="H129" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="C130" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="G130" t="s">
-        <v>237</v>
+        <v>110</v>
       </c>
       <c r="H130" t="s">
-        <v>270</v>
+        <v>119</v>
       </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.25">
@@ -3167,10 +3336,10 @@
         <v>274</v>
       </c>
       <c r="G131" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H131" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
@@ -3181,10 +3350,10 @@
         <v>274</v>
       </c>
       <c r="G132" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H132" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.25">
@@ -3195,24 +3364,27 @@
         <v>274</v>
       </c>
       <c r="G133" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H133" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="C134" t="s">
-        <v>274</v>
+        <v>195</v>
+      </c>
+      <c r="D134" t="s">
+        <v>285</v>
       </c>
       <c r="G134" t="s">
-        <v>104</v>
-      </c>
-      <c r="H134" t="s">
-        <v>105</v>
+        <v>147</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
@@ -3226,7 +3398,7 @@
         <v>147</v>
       </c>
       <c r="H135" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="136" spans="2:8" x14ac:dyDescent="0.25">
@@ -3240,7 +3412,7 @@
         <v>147</v>
       </c>
       <c r="H136" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="137" spans="2:8" x14ac:dyDescent="0.25">
@@ -3254,7 +3426,7 @@
         <v>147</v>
       </c>
       <c r="H137" t="s">
-        <v>171</v>
+        <v>196</v>
       </c>
     </row>
     <row r="138" spans="2:8" x14ac:dyDescent="0.25">
@@ -3268,7 +3440,7 @@
         <v>147</v>
       </c>
       <c r="H138" t="s">
-        <v>196</v>
+        <v>172</v>
       </c>
     </row>
     <row r="139" spans="2:8" x14ac:dyDescent="0.25">
@@ -3282,7 +3454,7 @@
         <v>147</v>
       </c>
       <c r="H139" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="140" spans="2:8" x14ac:dyDescent="0.25">
@@ -3296,7 +3468,7 @@
         <v>147</v>
       </c>
       <c r="H140" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="141" spans="2:8" x14ac:dyDescent="0.25">
@@ -3310,7 +3482,7 @@
         <v>147</v>
       </c>
       <c r="H141" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="142" spans="2:8" x14ac:dyDescent="0.25">
@@ -3324,7 +3496,7 @@
         <v>147</v>
       </c>
       <c r="H142" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="143" spans="2:8" x14ac:dyDescent="0.25">
@@ -3338,7 +3510,7 @@
         <v>147</v>
       </c>
       <c r="H143" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="144" spans="2:8" x14ac:dyDescent="0.25">
@@ -3352,7 +3524,7 @@
         <v>147</v>
       </c>
       <c r="H144" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
@@ -3366,7 +3538,7 @@
         <v>147</v>
       </c>
       <c r="H145" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.25">
@@ -3380,7 +3552,7 @@
         <v>147</v>
       </c>
       <c r="H146" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
@@ -3394,7 +3566,7 @@
         <v>147</v>
       </c>
       <c r="H147" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.25">
@@ -3408,7 +3580,7 @@
         <v>147</v>
       </c>
       <c r="H148" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.25">
@@ -3422,7 +3594,7 @@
         <v>147</v>
       </c>
       <c r="H149" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.25">
@@ -3436,7 +3608,7 @@
         <v>147</v>
       </c>
       <c r="H150" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
@@ -3450,7 +3622,7 @@
         <v>147</v>
       </c>
       <c r="H151" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
@@ -3464,7 +3636,7 @@
         <v>147</v>
       </c>
       <c r="H152" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
@@ -3478,7 +3650,7 @@
         <v>147</v>
       </c>
       <c r="H153" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
@@ -3492,7 +3664,7 @@
         <v>147</v>
       </c>
       <c r="H154" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
@@ -3500,13 +3672,16 @@
         <v>48</v>
       </c>
       <c r="C155" t="s">
-        <v>195</v>
+        <v>274</v>
+      </c>
+      <c r="D155" t="s">
+        <v>286</v>
       </c>
       <c r="G155" t="s">
         <v>147</v>
       </c>
       <c r="H155" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.25">
@@ -3520,7 +3695,7 @@
         <v>147</v>
       </c>
       <c r="H156" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="157" spans="2:8" x14ac:dyDescent="0.25">
@@ -3531,24 +3706,30 @@
         <v>274</v>
       </c>
       <c r="G157" t="s">
-        <v>147</v>
+        <v>124</v>
       </c>
       <c r="H157" t="s">
-        <v>168</v>
+        <v>127</v>
       </c>
     </row>
     <row r="158" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B158" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="C158" t="s">
         <v>274</v>
       </c>
+      <c r="E158" t="s">
+        <v>49</v>
+      </c>
+      <c r="F158" t="s">
+        <v>52</v>
+      </c>
       <c r="G158" t="s">
         <v>124</v>
       </c>
       <c r="H158" t="s">
-        <v>127</v>
+        <v>280</v>
       </c>
     </row>
     <row r="159" spans="2:8" x14ac:dyDescent="0.25">
@@ -3558,11 +3739,11 @@
       <c r="C159" t="s">
         <v>274</v>
       </c>
-      <c r="E159" t="s">
-        <v>49</v>
-      </c>
-      <c r="F159" t="s">
-        <v>52</v>
+      <c r="G159" t="s">
+        <v>124</v>
+      </c>
+      <c r="H159" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="160" spans="2:8" x14ac:dyDescent="0.25">
@@ -3694,6 +3875,9 @@
       <c r="C167" t="s">
         <v>6</v>
       </c>
+      <c r="D167" t="s">
+        <v>302</v>
+      </c>
       <c r="G167" t="s">
         <v>62</v>
       </c>
@@ -4038,6 +4222,9 @@
       <c r="C186" t="s">
         <v>192</v>
       </c>
+      <c r="D186" t="s">
+        <v>277</v>
+      </c>
       <c r="G186" t="s">
         <v>113</v>
       </c>
@@ -4052,6 +4239,9 @@
       <c r="C187" t="s">
         <v>192</v>
       </c>
+      <c r="D187" t="s">
+        <v>278</v>
+      </c>
       <c r="G187" t="s">
         <v>72</v>
       </c>
@@ -4065,6 +4255,9 @@
       </c>
       <c r="C188" t="s">
         <v>192</v>
+      </c>
+      <c r="D188" t="s">
+        <v>279</v>
       </c>
       <c r="G188" t="s">
         <v>62</v>

</xml_diff>